<commit_message>
I usualy use SVN. I want to slowly migrate over to GIT. Ive done alot of major changes since the last commit i think? Sooner or later i will compleatly migrate over, Blegh...  - Minor documentation updates to?  - Rubish movement implementation, much work to be done.  - Turrets need to be fixed becouse they dont like it when you move the ship?  - Engines can activate via 'E' key.  - Selection and DeSelection of ship via LMB.  - Game autosaves on exit or shutdown, and autoloads on game start but crashes if player is interacted with.  - REMEMBER THAT YOU NEED TO HAVE THE DATABASE RUNNING TO RUN THE GAME!!!  - Minor refactoring.  - Other things i dont remmember...
</commit_message>
<xml_diff>
--- a/assets/Documentation/Project Stark Interactive Matrix.xlsx
+++ b/assets/Documentation/Project Stark Interactive Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Ship</t>
   </si>
@@ -82,6 +82,9 @@
 Minor
 Dammage
 'Bounce'</t>
+  </si>
+  <si>
+    <t>v- Hits -&gt;</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="C2:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -454,6 +457,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:18" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>